<commit_message>
cleanup and finalizing for custom values
</commit_message>
<xml_diff>
--- a/custom_values.xlsx
+++ b/custom_values.xlsx
@@ -20,23 +20,44 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t xml:space="preserve">Value</t>
   </si>
   <si>
+    <t xml:space="preserve">Feel Free to update the Values in L column to change scenarios</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Score</t>
+  </si>
+  <si>
     <t xml:space="preserve">Potential Overall Weight</t>
   </si>
   <si>
+    <t xml:space="preserve">These values are used in the final score. They are multiples. Use the example to the right to see with your values </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Scenario 1: Projected 82 Overall with 9.92 Ras, and average of 12 on reports.</t>
+  </si>
+  <si>
     <t xml:space="preserve">RAS Weight</t>
   </si>
   <si>
+    <t xml:space="preserve">Scenario 2: Projected 75 Overall with 8.53 Ras, and average of 18 on reports.</t>
+  </si>
+  <si>
     <t xml:space="preserve">Report Weight</t>
   </si>
   <si>
+    <t xml:space="preserve">Scenario 3: Projected 71 Overall with 6.34 Ras, and average of 21 on reports.</t>
+  </si>
+  <si>
     <t xml:space="preserve">All Pro in Report</t>
   </si>
   <si>
+    <t xml:space="preserve">These values are in the report score. It looks for these certain words and adds them to a score.</t>
+  </si>
+  <si>
     <t xml:space="preserve">Sky High In Report</t>
   </si>
   <si>
@@ -65,6 +86,9 @@
   </si>
   <si>
     <t xml:space="preserve">Strategy Culture</t>
+  </si>
+  <si>
+    <t xml:space="preserve">These values are for the culture score. If a player has this culture it adds to their total score.</t>
   </si>
   <si>
     <t xml:space="preserve">Energetic Culture</t>
@@ -83,8 +107,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="General"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -108,20 +133,89 @@
       <family val="0"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF000000"/>
+        <bgColor rgb="FF003300"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="10">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="hair"/>
+      <right/>
+      <top style="hair"/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="hair"/>
+      <right style="hair"/>
+      <top style="hair"/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right/>
+      <top style="hair"/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right style="hair"/>
+      <top style="hair"/>
+      <bottom style="hair"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="hair"/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="hair"/>
+      <right style="hair"/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="hair"/>
+      <right/>
+      <top/>
+      <bottom style="hair"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="hair"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="hair"/>
+      <right style="hair"/>
+      <top/>
+      <bottom style="hair"/>
       <diagonal/>
     </border>
   </borders>
@@ -150,8 +244,60 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="14">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -172,10 +318,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B19"/>
+  <dimension ref="A1:L19"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
+      <selection pane="topLeft" activeCell="N21" activeCellId="0" sqref="N21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -187,152 +333,373 @@
       <c r="B1" s="0" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="F1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="0" t="n">
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="2" t="s">
         <v>2</v>
       </c>
     </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="6"/>
+      <c r="K2" s="6"/>
+      <c r="L2" s="7" t="n">
+        <f aca="false">SUM((82*B2)+(9.92*B3)+(12*B4))</f>
+        <v>225.6</v>
+      </c>
+    </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>2</v>
+      <c r="A3" s="8" t="s">
+        <v>6</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>5</v>
       </c>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
+      <c r="I3" s="6"/>
+      <c r="J3" s="6"/>
+      <c r="K3" s="6"/>
+      <c r="L3" s="7" t="n">
+        <f aca="false">SUM((75*B2)+(8.53*B3)+(18*B4))</f>
+        <v>210.65</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="0" t="n">
+      <c r="A4" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="10" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="0" t="n">
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="G4" s="11"/>
+      <c r="H4" s="11"/>
+      <c r="I4" s="11"/>
+      <c r="J4" s="11"/>
+      <c r="K4" s="11"/>
+      <c r="L4" s="12" t="n">
+        <f aca="false">SUM((71*B2)+(6.34*B3)+(21*B4))</f>
+        <v>194.7</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="4" t="n">
         <v>2</v>
       </c>
+      <c r="C5" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="13"/>
+      <c r="G5" s="13"/>
+      <c r="H5" s="13"/>
+      <c r="I5" s="13"/>
+      <c r="J5" s="13"/>
+      <c r="K5" s="13"/>
+      <c r="L5" s="13"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
-        <v>5</v>
+      <c r="A6" s="8" t="s">
+        <v>12</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>7</v>
       </c>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="13"/>
+      <c r="G6" s="13"/>
+      <c r="H6" s="13"/>
+      <c r="I6" s="13"/>
+      <c r="J6" s="13"/>
+      <c r="K6" s="13"/>
+      <c r="L6" s="13"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
-        <v>6</v>
+      <c r="A7" s="8" t="s">
+        <v>13</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>4</v>
       </c>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="13"/>
+      <c r="G7" s="13"/>
+      <c r="H7" s="13"/>
+      <c r="I7" s="13"/>
+      <c r="J7" s="13"/>
+      <c r="K7" s="13"/>
+      <c r="L7" s="13"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
-        <v>7</v>
+      <c r="A8" s="8" t="s">
+        <v>14</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>3</v>
       </c>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="13"/>
+      <c r="G8" s="13"/>
+      <c r="H8" s="13"/>
+      <c r="I8" s="13"/>
+      <c r="J8" s="13"/>
+      <c r="K8" s="13"/>
+      <c r="L8" s="13"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
-        <v>8</v>
+      <c r="A9" s="8" t="s">
+        <v>15</v>
       </c>
       <c r="B9" s="0" t="n">
         <v>2</v>
       </c>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="13"/>
+      <c r="G9" s="13"/>
+      <c r="H9" s="13"/>
+      <c r="I9" s="13"/>
+      <c r="J9" s="13"/>
+      <c r="K9" s="13"/>
+      <c r="L9" s="13"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
-        <v>9</v>
+      <c r="A10" s="8" t="s">
+        <v>16</v>
       </c>
       <c r="B10" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="13"/>
+      <c r="H10" s="13"/>
+      <c r="I10" s="13"/>
+      <c r="J10" s="13"/>
+      <c r="K10" s="13"/>
+      <c r="L10" s="13"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
-        <v>10</v>
+      <c r="A11" s="8" t="s">
+        <v>17</v>
       </c>
       <c r="B11" s="0" t="n">
         <v>10</v>
       </c>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="13"/>
+      <c r="G11" s="13"/>
+      <c r="H11" s="13"/>
+      <c r="I11" s="13"/>
+      <c r="J11" s="13"/>
+      <c r="K11" s="13"/>
+      <c r="L11" s="13"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
-        <v>11</v>
+      <c r="A12" s="8" t="s">
+        <v>18</v>
       </c>
       <c r="B12" s="0" t="n">
         <v>7</v>
       </c>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="13"/>
+      <c r="G12" s="13"/>
+      <c r="H12" s="13"/>
+      <c r="I12" s="13"/>
+      <c r="J12" s="13"/>
+      <c r="K12" s="13"/>
+      <c r="L12" s="13"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
-        <v>12</v>
+      <c r="A13" s="8" t="s">
+        <v>19</v>
       </c>
       <c r="B13" s="0" t="n">
         <v>3</v>
       </c>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="13"/>
+      <c r="G13" s="13"/>
+      <c r="H13" s="13"/>
+      <c r="I13" s="13"/>
+      <c r="J13" s="13"/>
+      <c r="K13" s="13"/>
+      <c r="L13" s="13"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="B14" s="0" t="n">
+      <c r="A14" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" s="10" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="B15" s="0" t="n">
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="13"/>
+      <c r="G14" s="13"/>
+      <c r="H14" s="13"/>
+      <c r="I14" s="13"/>
+      <c r="J14" s="13"/>
+      <c r="K14" s="13"/>
+      <c r="L14" s="13"/>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A15" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B15" s="4" t="n">
         <v>15</v>
       </c>
+      <c r="C15" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="13"/>
+      <c r="G15" s="13"/>
+      <c r="H15" s="13"/>
+      <c r="I15" s="13"/>
+      <c r="J15" s="13"/>
+      <c r="K15" s="13"/>
+      <c r="L15" s="13"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
-        <v>15</v>
+      <c r="A16" s="8" t="s">
+        <v>23</v>
       </c>
       <c r="B16" s="0" t="n">
         <v>2</v>
       </c>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="13"/>
+      <c r="G16" s="13"/>
+      <c r="H16" s="13"/>
+      <c r="I16" s="13"/>
+      <c r="J16" s="13"/>
+      <c r="K16" s="13"/>
+      <c r="L16" s="13"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
-        <v>16</v>
+      <c r="A17" s="8" t="s">
+        <v>24</v>
       </c>
       <c r="B17" s="0" t="n">
         <v>5</v>
       </c>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="13"/>
+      <c r="G17" s="13"/>
+      <c r="H17" s="13"/>
+      <c r="I17" s="13"/>
+      <c r="J17" s="13"/>
+      <c r="K17" s="13"/>
+      <c r="L17" s="13"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
-        <v>17</v>
+      <c r="A18" s="8" t="s">
+        <v>25</v>
       </c>
       <c r="B18" s="0" t="n">
         <v>5</v>
       </c>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="13"/>
+      <c r="G18" s="13"/>
+      <c r="H18" s="13"/>
+      <c r="I18" s="13"/>
+      <c r="J18" s="13"/>
+      <c r="K18" s="13"/>
+      <c r="L18" s="13"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="B19" s="0" t="n">
+      <c r="A19" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B19" s="10" t="n">
         <v>15</v>
       </c>
+      <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="13"/>
+      <c r="G19" s="13"/>
+      <c r="H19" s="13"/>
+      <c r="I19" s="13"/>
+      <c r="J19" s="13"/>
+      <c r="K19" s="13"/>
+      <c r="L19" s="13"/>
     </row>
   </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="F1:K1"/>
+    <mergeCell ref="C2:E4"/>
+    <mergeCell ref="F2:K2"/>
+    <mergeCell ref="F3:K3"/>
+    <mergeCell ref="F4:K4"/>
+    <mergeCell ref="C5:E14"/>
+    <mergeCell ref="C15:E19"/>
+  </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>